<commit_message>
Changed "DESCRIBE" to "CONSTRUCT" in sparql query.  it is more reliable than describe!
</commit_message>
<xml_diff>
--- a/Documents/IndoPacific/indoPacificTemplate_v8.xlsx
+++ b/Documents/IndoPacific/indoPacificTemplate_v8.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9200" yWindow="1740" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-12180" yWindow="-22040" windowWidth="16740" windowHeight="22660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -30,835 +30,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Eric Crandall</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>The "local" accession number that you use for your laboratory's database. This number should link EXACTLY to the genetic data you are providing for this sample. It must be unique among the numbers that your lab is providing.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Firstname Lastname (the PI on the grant that generated this data)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Most commonly used acronym for your university, agency or institution</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Granting body and grant number, can be in a delimited list.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Specimen voucher ID</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Photos, videos etc of the individual. From Darwincore: A list (concatenated and separated) of identifiers (publication, global unique identifier, URI,DOI) of media associated with the Occurrence.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Eric Crandall:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Any associated publications or references pertaining to this individual or its derivative tissues or sequences. The first place it was published is particularly relevant. From Darwincore: A list (concatenated and separated) of identifiers (publication, bibliographic reference, global unique identifier, URI) of literature associated with the Occurrence.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>A list (concatenated and separated) of preparations and preservation methods for a specimen. Example: "95% EtOH"; "Frozen"</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>A list (concatenated and separated) of previous assignments of names to the Occurrence.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>The age class or life stage of the biological individual(s) at the time the Occurrence was recorded. Recommended best practice is to use a controlled vocabulary.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>In Grams. Referring to the weight of the organism from which the sample was derived</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>In Centimeters. Referring to the length of the organism from which the sample was derived</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>The sex of the biological individual(s) represented in the Occurrence. Recommended best practice is to use a controlled vocabulary. See associated list on "lists" tab.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>The process by which the biological individual(s) represented in the Occurrence became established at the location. Recommended best practice is to use a controlled vocabulary. See associated list in "lists" tab.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>A list (concatenated and separated) of identifiers (publication, global unique identifier, URI) of genetic sequence information associated with the Occurrence. Links to Genbank or DRYAD entries.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Any other relevant comments or notes about the sample itself.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Q1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>YYYY (the year collected)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="R1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>MM (the month collected)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="S1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>DD (the day collected)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="T1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Please include any permit information (agency, permit#, etc) as a text string</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Habitat from which the sample was collected. Please pick from the associated list in "lists" tab.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="V1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Information about the microhabitat from which the sample was collected. E.g. Forereef, coral head
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Substrate from which the individual was sampled. This could be abiotic or biotic (host organism).</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="X1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Brief description of how the sample was taken. From Darwincore: The name of, reference to, or description of the method or protocol used during an Event.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Y1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>In Meters. Use with maximum depth to bracket the range of depth at which the sample was taken. In meters (positive values below surface)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Z1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>In Meters. Use with minimum depth to bracket the range of depth at which the sample was taken. In meters (positive values below surface)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AA1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>In Meters. Use with maximum distance above surface to bracket the range of height at which the sample was taken in meters (positive values above surface)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AB1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>In Meters. Use with minimum distance above surface to bracket the range of height at which the sample was taken in meters (positive values above surface)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AC1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>A list (concatenated and separated) of hosts/parasites/symbionts of the sampled individual.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AD1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Any notes taken in the field, or a link to those notes: population size, ecological info, etc.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AE1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>A text string for notes that were written on the original label during collection</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AF1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Full Name (can be list -- primary collector first, separate list by semicolons)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AG1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Decimal Degrees. If you don't have this information, you must enter something into the locality field to the best known precision.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AH1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Decimal Degrees. If you don't have this information, you must enter something into the locality field to the best known precision.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AI1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>In meters.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AJ1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>A description or reference to the methods used to determine the spatial footprint, coordinates, and uncertainties (e.g. GPS, Approximated from Google Maps, Based on locality name search in Google Maps (Ben Morris' script) etc.)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AK1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>The country where the sample was found. Must be found in associated list in "lists" tab.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AL1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>The state or province where the sample was found.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AM1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>The island where the sample was found.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AN1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>The island group or archipelago where the sample was found.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AP1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Eric Crandall:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Morphology, Genetic, Other.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AQ1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Full Name (A list (concatenated and separated) of names of people, groups, or organizations who assigned the Taxon to the subject.)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AR1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>YYYY</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AS1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>MM</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AT1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>DD</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AU1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>The full scientific name of the genus in which the taxon is classified.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AV1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>The name of the first or species epithet of the scientificName.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AW1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>The name of the lowest or terminal infraspecific epithet of the scientificName, excluding any rank designation.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AX1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Common name and/or native name</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AY1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>The full scientific name of the phylum in which the taxon is classified. Required.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AZ1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>The full scientific name of the class in which the taxon is classified.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BA1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>The full scientific name of the order in which the taxon is classified.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BB1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>The full scientific name of the family in which the taxon is classified.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BC1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Comments or notes about the taxon or name.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BD1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Identification # (AphiaID) for Worms database (http://www.marinespecies.org/). Please try to provide this or the genus/species.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BE1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>A list (concatenated and separated) of the tissue types sampled from this individual, together with any tissue identifiers that were assigned to them</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BF1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>A platename where the DNA extract is stored</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BG1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>The well on the plate where the DNA extract is stored</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BH1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>A unique identifier for the extraction (other than plate or well)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BI1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Other identifiers for this tissue.  E.g. tissue originated in another institution.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BJ1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>A list (concatenated and separated) of further identifiers for the container which holds the material sample.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="469">
   <si>
     <t>Samples Tab</t>
   </si>
@@ -1163,6 +336,9 @@
     <t>microHabitat</t>
   </si>
   <si>
+    <t>Information about the microhabitat from which the sample was collected. Please pick from the associated list in "lists" tab. (Currently working with Chris Bird for a list)</t>
+  </si>
+  <si>
     <t>Reef Slope</t>
   </si>
   <si>
@@ -2243,6 +1419,9 @@
     <t>Yemen</t>
   </si>
   <si>
+    <t>Please fill out each field in the "Samples" tab as completely as possible. Fields in red are required (data cannot be uploaded to the database without these fields). For locality, you must either provide a locality description that could be looked up in Google Maps (the locality may be as precise as "Sanur Lagoon" or as broad as "Pacific Ocean") OR latitude and longitude coordinates in decimal degrees. Fields in yellow are highly recommended (you will receive a warning from the program if you do not provide this information). An example entry is provided, please delete this entry before uploading your data. If you have more than one entry to a field (i.e. a list of publications), please delimit your list with semicolons (;).  Fields in the samples tab may be re-arranged in any order SO LONG AS YOU DON'T CHANGE THE FIELD NAMES.</t>
+  </si>
+  <si>
     <t>American Samoa</t>
   </si>
   <si>
@@ -2252,22 +1431,13 @@
     <t>version 8</t>
   </si>
   <si>
+    <t>January 2nd, 2014</t>
+  </si>
+  <si>
     <t>Database_Fields&amp;Notes  Tab</t>
   </si>
   <si>
     <t>Lists Tab</t>
-  </si>
-  <si>
-    <t>Information about the microhabitat from which the sample was collected. E.g. Forereef, coral head</t>
-  </si>
-  <si>
-    <t>Please fill out each field in the "Samples" tab as completely as possible. Fields in red are required (data cannot be uploaded to the database without these fields). For locality, you must either provide a locality description that could be looked up in Google Maps (the locality may be as precise as "Sanur Lagoon" or as broad as "Pacific Ocean") OR latitude and longitude coordinates in decimal degrees. Fields in yellow are highly recommended (you will receive a warning from the program if you do not provide this information). Fields in purple have a list of "controlled vocabulary" associated with them that you may find in the "lists" tab. An example entry is provided, please delete this entry before uploading your data. If you have more than one entry to a field (i.e. a list of publications), please delimit your list with semicolons (;).  Fields in the samples tab may be re-arranged in any order SO LONG AS YOU DON'T CHANGE THE FIELD NAMES.</t>
-  </si>
-  <si>
-    <t>January 5th, 2014</t>
-  </si>
-  <si>
-    <t>Please contact Eric Crandall (eric.darvish@gmail.com) if you have any questions about this template</t>
   </si>
 </sst>
 </file>
@@ -2277,7 +1447,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="80" x14ac:knownFonts="1">
+  <fonts count="77" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2325,6 +1495,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
@@ -2693,30 +1869,6 @@
       <u/>
       <sz val="10"/>
       <color theme="11"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -3258,44 +2410,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3321,185 +2459,188 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="36" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="37" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="27" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="56" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="59" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="39" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="39" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="61" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="62" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="63" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="64" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="65" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="66" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="66" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="67" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="68" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="71" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="72" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="72" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="36" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="57" fillId="36" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="70" fillId="46" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="73" fillId="48" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="71" fillId="46" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="37" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="74" fillId="48" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="37" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3508,41 +2649,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="49" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="33" fillId="49" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="49" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="49" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="79" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3553,13 +2685,6 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3570,13 +2695,6 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3906,74 +3024,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A2:A15"/>
+  <dimension ref="A2:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="144.33203125" customWidth="1"/>
+    <col min="1" max="1" width="77.6640625" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" ht="16" customHeight="1">
-      <c r="A2" s="85" t="s">
+    <row r="2" spans="1:1" ht="12.75" customHeight="1">
+      <c r="A2" s="83" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="12.75" customHeight="1">
+      <c r="A3" s="83" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="12.75" customHeight="1">
+      <c r="A4" s="84" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="12.75" customHeight="1">
+      <c r="A5" s="82"/>
+    </row>
+    <row r="6" spans="1:1" ht="12">
+      <c r="A6" s="81" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="108">
+      <c r="A7" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="19" customHeight="1">
-      <c r="A3" s="85" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="19" customHeight="1">
-      <c r="A4" s="86" t="s">
+    <row r="8" spans="1:1" ht="12"/>
+    <row r="9" spans="1:1" ht="12">
+      <c r="A9" s="81" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="36">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="12"/>
+    <row r="12" spans="1:1" ht="12">
+      <c r="A12" s="80" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="12.75" customHeight="1">
-      <c r="A5" s="79"/>
-    </row>
-    <row r="6" spans="1:1" ht="15">
-      <c r="A6" s="83" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="90">
-      <c r="A7" s="82" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="12"/>
-    <row r="9" spans="1:1" ht="15">
-      <c r="A9" s="83" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="30">
-      <c r="A10" s="82" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="15">
-      <c r="A11" s="82"/>
-    </row>
-    <row r="12" spans="1:1" ht="15">
-      <c r="A12" s="84" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="16" customHeight="1">
-      <c r="A13" s="82" t="s">
+    <row r="13" spans="1:1" ht="12.75" customHeight="1">
+      <c r="A13" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="17" customHeight="1">
-      <c r="A15" t="s">
-        <v>469</v>
       </c>
     </row>
   </sheetData>
@@ -3988,236 +3098,219 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BJ21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T3" sqref="T3"/>
+      <selection pane="bottomLeft" activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.5" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" customWidth="1"/>
     <col min="7" max="8" width="22.33203125" customWidth="1"/>
     <col min="9" max="9" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" customWidth="1"/>
-    <col min="14" max="14" width="19.1640625" customWidth="1"/>
-    <col min="15" max="15" width="20.33203125" customWidth="1"/>
-    <col min="16" max="16" width="18.5" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" customWidth="1"/>
-    <col min="19" max="19" width="16.6640625" customWidth="1"/>
+    <col min="13" max="13" width="29.6640625" customWidth="1"/>
+    <col min="14" max="14" width="17.33203125" customWidth="1"/>
     <col min="20" max="20" width="18.1640625" style="17" customWidth="1"/>
     <col min="21" max="21" width="19.5" style="17" customWidth="1"/>
-    <col min="22" max="22" width="15.83203125" customWidth="1"/>
-    <col min="23" max="23" width="15" customWidth="1"/>
-    <col min="24" max="24" width="18" customWidth="1"/>
-    <col min="26" max="26" width="21.1640625" customWidth="1"/>
-    <col min="27" max="27" width="38" customWidth="1"/>
-    <col min="28" max="28" width="35.1640625" customWidth="1"/>
-    <col min="29" max="29" width="17" customWidth="1"/>
-    <col min="31" max="31" width="16" customWidth="1"/>
-    <col min="33" max="33" width="16.1640625" customWidth="1"/>
-    <col min="34" max="34" width="17" customWidth="1"/>
-    <col min="35" max="35" width="25.6640625" customWidth="1"/>
-    <col min="36" max="36" width="20.83203125" customWidth="1"/>
+    <col min="22" max="22" width="32.33203125" customWidth="1"/>
     <col min="42" max="42" width="15.83203125" customWidth="1"/>
     <col min="48" max="49" width="14.6640625" customWidth="1"/>
     <col min="50" max="50" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" s="75" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="80" t="s">
+    <row r="1" spans="1:62" s="76" customFormat="1" ht="15" customHeight="1">
+      <c r="A1" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="68" t="s">
+      <c r="D1" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="68" t="s">
+      <c r="F1" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="68" t="s">
+      <c r="H1" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="68" t="s">
+      <c r="I1" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="68" t="s">
+      <c r="J1" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="68" t="s">
+      <c r="K1" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="68" t="s">
+      <c r="L1" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="77" t="s">
+      <c r="M1" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="77" t="s">
+      <c r="N1" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="O1" s="68" t="s">
+      <c r="O1" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="P1" s="68" t="s">
+      <c r="P1" s="69" t="s">
         <v>76</v>
       </c>
-      <c r="Q1" s="70" t="s">
+      <c r="Q1" s="71" t="s">
         <v>81</v>
       </c>
-      <c r="R1" s="68" t="s">
+      <c r="R1" s="69" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="68" t="s">
+      <c r="S1" s="69" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="71" t="s">
+      <c r="T1" s="72" t="s">
         <v>92</v>
       </c>
-      <c r="U1" s="76" t="s">
+      <c r="U1" s="77" t="s">
         <v>96</v>
       </c>
-      <c r="V1" s="68" t="s">
+      <c r="V1" s="69" t="s">
         <v>100</v>
       </c>
-      <c r="W1" s="68" t="s">
-        <v>102</v>
-      </c>
-      <c r="X1" s="68" t="s">
-        <v>106</v>
-      </c>
-      <c r="Y1" s="68" t="s">
-        <v>110</v>
-      </c>
-      <c r="Z1" s="68" t="s">
-        <v>114</v>
-      </c>
-      <c r="AA1" s="68" t="s">
-        <v>118</v>
-      </c>
-      <c r="AB1" s="68" t="s">
-        <v>121</v>
-      </c>
-      <c r="AC1" s="68" t="s">
-        <v>124</v>
-      </c>
-      <c r="AD1" s="68" t="s">
-        <v>128</v>
-      </c>
-      <c r="AE1" s="68" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF1" s="68" t="s">
-        <v>135</v>
-      </c>
-      <c r="AG1" s="68" t="s">
-        <v>140</v>
-      </c>
-      <c r="AH1" s="68" t="s">
-        <v>145</v>
-      </c>
-      <c r="AI1" s="70" t="s">
-        <v>147</v>
-      </c>
-      <c r="AJ1" s="70" t="s">
-        <v>150</v>
-      </c>
-      <c r="AK1" s="72" t="s">
-        <v>154</v>
-      </c>
-      <c r="AL1" s="68" t="s">
-        <v>158</v>
-      </c>
-      <c r="AM1" s="68" t="s">
-        <v>162</v>
-      </c>
-      <c r="AN1" s="68" t="s">
-        <v>165</v>
-      </c>
-      <c r="AO1" s="73" t="s">
-        <v>169</v>
-      </c>
-      <c r="AP1" s="70" t="s">
-        <v>176</v>
-      </c>
-      <c r="AQ1" s="68" t="s">
-        <v>181</v>
-      </c>
-      <c r="AR1" s="68" t="s">
-        <v>184</v>
-      </c>
-      <c r="AS1" s="68" t="s">
-        <v>187</v>
-      </c>
-      <c r="AT1" s="68" t="s">
-        <v>190</v>
-      </c>
-      <c r="AU1" s="70" t="s">
-        <v>194</v>
-      </c>
-      <c r="AV1" s="70" t="s">
-        <v>200</v>
-      </c>
-      <c r="AW1" s="68" t="s">
-        <v>204</v>
-      </c>
-      <c r="AX1" s="68" t="s">
-        <v>207</v>
-      </c>
-      <c r="AY1" s="74" t="s">
-        <v>211</v>
-      </c>
-      <c r="AZ1" s="68" t="s">
-        <v>216</v>
-      </c>
-      <c r="BA1" s="68" t="s">
-        <v>221</v>
-      </c>
-      <c r="BB1" s="68" t="s">
-        <v>225</v>
-      </c>
-      <c r="BC1" s="68" t="s">
-        <v>229</v>
-      </c>
-      <c r="BD1" s="70" t="s">
-        <v>232</v>
-      </c>
-      <c r="BE1" s="68" t="s">
-        <v>238</v>
-      </c>
-      <c r="BF1" s="68" t="s">
-        <v>242</v>
-      </c>
-      <c r="BG1" s="68" t="s">
-        <v>246</v>
-      </c>
-      <c r="BH1" s="68" t="s">
-        <v>250</v>
-      </c>
-      <c r="BI1" s="68" t="s">
-        <v>253</v>
-      </c>
-      <c r="BJ1" s="68" t="s">
-        <v>256</v>
+      <c r="W1" s="69" t="s">
+        <v>103</v>
+      </c>
+      <c r="X1" s="69" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y1" s="69" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z1" s="69" t="s">
+        <v>115</v>
+      </c>
+      <c r="AA1" s="69" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB1" s="69" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC1" s="69" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD1" s="69" t="s">
+        <v>129</v>
+      </c>
+      <c r="AE1" s="69" t="s">
+        <v>133</v>
+      </c>
+      <c r="AF1" s="69" t="s">
+        <v>136</v>
+      </c>
+      <c r="AG1" s="69" t="s">
+        <v>141</v>
+      </c>
+      <c r="AH1" s="69" t="s">
+        <v>146</v>
+      </c>
+      <c r="AI1" s="71" t="s">
+        <v>148</v>
+      </c>
+      <c r="AJ1" s="71" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK1" s="73" t="s">
+        <v>155</v>
+      </c>
+      <c r="AL1" s="69" t="s">
+        <v>159</v>
+      </c>
+      <c r="AM1" s="69" t="s">
+        <v>163</v>
+      </c>
+      <c r="AN1" s="69" t="s">
+        <v>166</v>
+      </c>
+      <c r="AO1" s="74" t="s">
+        <v>170</v>
+      </c>
+      <c r="AP1" s="71" t="s">
+        <v>177</v>
+      </c>
+      <c r="AQ1" s="69" t="s">
+        <v>182</v>
+      </c>
+      <c r="AR1" s="69" t="s">
+        <v>185</v>
+      </c>
+      <c r="AS1" s="69" t="s">
+        <v>188</v>
+      </c>
+      <c r="AT1" s="69" t="s">
+        <v>191</v>
+      </c>
+      <c r="AU1" s="71" t="s">
+        <v>195</v>
+      </c>
+      <c r="AV1" s="71" t="s">
+        <v>201</v>
+      </c>
+      <c r="AW1" s="69" t="s">
+        <v>205</v>
+      </c>
+      <c r="AX1" s="69" t="s">
+        <v>208</v>
+      </c>
+      <c r="AY1" s="75" t="s">
+        <v>212</v>
+      </c>
+      <c r="AZ1" s="69" t="s">
+        <v>217</v>
+      </c>
+      <c r="BA1" s="69" t="s">
+        <v>222</v>
+      </c>
+      <c r="BB1" s="69" t="s">
+        <v>226</v>
+      </c>
+      <c r="BC1" s="69" t="s">
+        <v>230</v>
+      </c>
+      <c r="BD1" s="71" t="s">
+        <v>233</v>
+      </c>
+      <c r="BE1" s="69" t="s">
+        <v>239</v>
+      </c>
+      <c r="BF1" s="69" t="s">
+        <v>243</v>
+      </c>
+      <c r="BG1" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="BH1" s="69" t="s">
+        <v>251</v>
+      </c>
+      <c r="BI1" s="69" t="s">
+        <v>254</v>
+      </c>
+      <c r="BJ1" s="69" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:62" ht="15" customHeight="1">
@@ -4246,7 +3339,7 @@
         <v>47</v>
       </c>
       <c r="I2" s="41" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="J2" s="41" t="s">
         <v>56</v>
@@ -4285,13 +3378,13 @@
         <v>99</v>
       </c>
       <c r="V2" s="41" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="W2" s="41" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="X2" s="41" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="Y2" s="41">
         <v>20</v>
@@ -4302,14 +3395,14 @@
       <c r="AA2" s="41"/>
       <c r="AB2" s="41"/>
       <c r="AC2" s="41" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AD2" s="41" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AE2" s="41"/>
       <c r="AF2" s="41" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="AG2" s="41">
         <v>-8.6992250000000002</v>
@@ -4321,28 +3414,28 @@
         <v>100</v>
       </c>
       <c r="AJ2" s="41" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AK2" s="41" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AL2" s="41" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AM2" s="41" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AN2" s="41" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AO2" s="41" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AP2" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="AQ2" s="41" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="AR2" s="41">
         <v>2006</v>
@@ -4354,46 +3447,46 @@
         <v>21</v>
       </c>
       <c r="AU2" s="41" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AV2" s="41" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AW2" s="41"/>
       <c r="AX2" s="41" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AY2" s="41" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AZ2" s="41" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="BA2" s="41" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="BB2" s="41" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="BC2" s="41"/>
       <c r="BD2" s="41">
         <v>207610</v>
       </c>
       <c r="BE2" s="41" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="BF2" s="41" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="BG2" s="41" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="BH2" s="41" t="s">
         <v>18</v>
       </c>
       <c r="BI2" s="41"/>
       <c r="BJ2" s="41" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:62" ht="15" customHeight="1">
@@ -4421,8 +3514,8 @@
       <c r="U8" s="23"/>
     </row>
     <row r="9" spans="1:62" ht="15" customHeight="1">
-      <c r="T9"/>
-      <c r="U9"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="23"/>
     </row>
     <row r="10" spans="1:62" ht="15" customHeight="1">
       <c r="T10" s="23"/>
@@ -4474,46 +3567,44 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="26">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="27">
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Country">
           <x14:formula1>
             <xm:f>Lists!$F:$F</xm:f>
           </x14:formula1>
-          <xm:sqref>AK1:AK8 AK10:AK1048576</xm:sqref>
+          <xm:sqref>AK1:AK1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lists!$B:$B</xm:f>
           </x14:formula1>
-          <xm:sqref>U1:U8 U10:U1048576</xm:sqref>
+          <xm:sqref>U1:U1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>Lists!$C:$C</xm:f>
           </x14:formula1>
-          <xm:sqref>M1:M8 M10:M1048576</xm:sqref>
+          <xm:sqref>M1:M1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lists!$D:$D</xm:f>
           </x14:formula1>
-          <xm:sqref>N1:N8 N10:N1048576</xm:sqref>
+          <xm:sqref>N1:N1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unknown Phylum">
           <x14:formula1>
             <xm:f>Lists!$G:$G</xm:f>
           </x14:formula1>
-          <xm:sqref>AY1:AY8 AY10:AY1048576</xm:sqref>
+          <xm:sqref>AY1:AY1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lists!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>AP1:AP8 AP10:AP1048576</xm:sqref>
+          <xm:sqref>AP1:AP1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="validationFailed">
           <x14:formula1>
@@ -4562,6 +3653,12 @@
             <xm:f>Lists!E2:E4</xm:f>
           </x14:formula1>
           <xm:sqref>J8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lists!E2:E4</xm:f>
+          </x14:formula1>
+          <xm:sqref>J9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
@@ -4646,12 +3743,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -4660,8 +3756,8 @@
     <col min="2" max="2" width="52.83203125" style="34" customWidth="1"/>
     <col min="3" max="3" width="24.1640625" style="34" customWidth="1"/>
     <col min="4" max="4" width="24.83203125" style="34" customWidth="1"/>
-    <col min="5" max="5" width="36.5" style="34" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="27.5" style="34" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="36.5" style="34" customWidth="1"/>
+    <col min="6" max="6" width="27.5" style="34" customWidth="1"/>
     <col min="7" max="7" width="131.5" style="34" customWidth="1"/>
     <col min="8" max="8" width="108.5" style="10" customWidth="1"/>
     <col min="9" max="9" width="33.5" customWidth="1"/>
@@ -4992,7 +4088,7 @@
         <v>64</v>
       </c>
       <c r="C14" s="55"/>
-      <c r="D14" s="78" t="s">
+      <c r="D14" s="79" t="s">
         <v>53</v>
       </c>
       <c r="E14" s="55" t="s">
@@ -5218,11 +4314,11 @@
       <c r="F23" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="G23" s="81" t="s">
-        <v>466</v>
+      <c r="G23" s="61" t="s">
+        <v>101</v>
       </c>
       <c r="H23" s="46" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I23" s="50"/>
     </row>
@@ -5231,21 +4327,21 @@
         <v>80</v>
       </c>
       <c r="B24" s="61" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C24" s="61"/>
       <c r="D24" s="61"/>
       <c r="E24" s="61" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F24" s="61" t="s">
         <v>16</v>
       </c>
       <c r="G24" s="61" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H24" s="46" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I24" s="50"/>
     </row>
@@ -5254,21 +4350,21 @@
         <v>80</v>
       </c>
       <c r="B25" s="61" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C25" s="61"/>
       <c r="D25" s="61"/>
       <c r="E25" s="61" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F25" s="61" t="s">
         <v>16</v>
       </c>
       <c r="G25" s="61" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H25" s="46" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I25" s="50"/>
     </row>
@@ -5277,20 +4373,20 @@
         <v>80</v>
       </c>
       <c r="B26" s="61" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C26" s="61"/>
       <c r="D26" s="61" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E26" s="61" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F26" s="61" t="s">
         <v>16</v>
       </c>
       <c r="G26" s="61" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H26" s="46">
         <v>20</v>
@@ -5302,20 +4398,20 @@
         <v>80</v>
       </c>
       <c r="B27" s="61" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C27" s="61"/>
       <c r="D27" s="61" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E27" s="61" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F27" s="61" t="s">
         <v>16</v>
       </c>
       <c r="G27" s="61" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H27" s="46">
         <v>1</v>
@@ -5327,20 +4423,20 @@
         <v>80</v>
       </c>
       <c r="B28" s="61" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C28" s="61"/>
       <c r="D28" s="61" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E28" s="61" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F28" s="61" t="s">
         <v>16</v>
       </c>
       <c r="G28" s="61" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H28" s="46"/>
       <c r="I28" s="50"/>
@@ -5350,20 +4446,20 @@
         <v>80</v>
       </c>
       <c r="B29" s="61" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C29" s="61"/>
       <c r="D29" s="61" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E29" s="61" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F29" s="61" t="s">
         <v>16</v>
       </c>
       <c r="G29" s="61" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H29" s="46"/>
       <c r="I29" s="50"/>
@@ -5373,21 +4469,21 @@
         <v>80</v>
       </c>
       <c r="B30" s="31" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C30" s="31"/>
       <c r="D30" s="31"/>
       <c r="E30" s="31" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F30" s="31" t="s">
         <v>16</v>
       </c>
       <c r="G30" s="61" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H30" s="37" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I30" s="35"/>
     </row>
@@ -5396,21 +4492,21 @@
         <v>80</v>
       </c>
       <c r="B31" s="61" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C31" s="61"/>
       <c r="D31" s="61"/>
       <c r="E31" s="61" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F31" s="61" t="s">
         <v>16</v>
       </c>
       <c r="G31" s="61" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H31" s="46" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I31" s="50"/>
     </row>
@@ -5419,18 +4515,18 @@
         <v>80</v>
       </c>
       <c r="B32" s="61" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C32" s="61"/>
       <c r="D32" s="61"/>
       <c r="E32" s="61" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F32" s="61" t="s">
         <v>16</v>
       </c>
       <c r="G32" s="61" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H32" s="46"/>
       <c r="I32" s="50"/>
@@ -5440,45 +4536,45 @@
         <v>80</v>
       </c>
       <c r="B33" s="61" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C33" s="61"/>
       <c r="D33" s="61"/>
       <c r="E33" s="61" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F33" s="61" t="s">
         <v>16</v>
       </c>
       <c r="G33" s="61" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H33" s="46" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I33" s="50"/>
     </row>
     <row r="34" spans="1:9" ht="14">
       <c r="A34" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H34" s="59">
         <v>-8.6992250000000002</v>
@@ -5487,25 +4583,25 @@
     </row>
     <row r="35" spans="1:9" ht="14">
       <c r="A35" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H35" s="59">
         <v>115.268333</v>
@@ -5514,10 +4610,10 @@
     </row>
     <row r="36" spans="1:9" ht="14">
       <c r="A36" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>82</v>
@@ -5526,13 +4622,13 @@
         <v>83</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H36" s="59">
         <v>100</v>
@@ -5541,10 +4637,10 @@
     </row>
     <row r="37" spans="1:9" ht="27.75" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>82</v>
@@ -5553,207 +4649,207 @@
         <v>83</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H37" s="59" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I37" s="50"/>
     </row>
     <row r="38" spans="1:9" ht="14">
       <c r="A38" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H38" s="59" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I38" s="50"/>
     </row>
     <row r="39" spans="1:9" ht="14">
       <c r="A39" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H39" s="59" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I39" s="50"/>
     </row>
     <row r="40" spans="1:9" ht="14">
       <c r="A40" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H40" s="59" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I40" s="50"/>
     </row>
     <row r="41" spans="1:9" ht="14">
       <c r="A41" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H41" s="59" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I41" s="50"/>
     </row>
     <row r="42" spans="1:9" ht="14">
       <c r="A42" s="60" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B42" s="60" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C42" s="60" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D42" s="60" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E42" s="60" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F42" s="60" t="s">
         <v>16</v>
       </c>
       <c r="G42" s="60" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H42" s="64" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I42" s="26"/>
     </row>
     <row r="43" spans="1:9" s="30" customFormat="1">
       <c r="A43" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B43" s="40" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D43" s="40" t="s">
         <v>83</v>
       </c>
       <c r="E43" s="40" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F43" s="40" t="s">
         <v>16</v>
       </c>
       <c r="G43" s="40" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H43" s="48" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I43" s="50"/>
     </row>
     <row r="44" spans="1:9" ht="27.75" customHeight="1">
       <c r="A44" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B44" s="40" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C44" s="40"/>
       <c r="D44" s="40"/>
       <c r="E44" s="40" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F44" s="40" t="s">
         <v>16</v>
       </c>
       <c r="G44" s="40" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H44" s="48" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I44" s="50"/>
     </row>
     <row r="45" spans="1:9" ht="14">
       <c r="A45" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B45" s="40" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C45" s="40"/>
       <c r="D45" s="40"/>
       <c r="E45" s="40" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F45" s="40" t="s">
         <v>16</v>
       </c>
       <c r="G45" s="40" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H45" s="48">
         <v>2006</v>
@@ -5762,21 +4858,21 @@
     </row>
     <row r="46" spans="1:9" ht="14">
       <c r="A46" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B46" s="40" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C46" s="40"/>
       <c r="D46" s="40"/>
       <c r="E46" s="40" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F46" s="40" t="s">
         <v>16</v>
       </c>
       <c r="G46" s="40" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H46" s="48">
         <v>10</v>
@@ -5785,21 +4881,21 @@
     </row>
     <row r="47" spans="1:9" ht="14">
       <c r="A47" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B47" s="40" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C47" s="40"/>
       <c r="D47" s="40"/>
       <c r="E47" s="40" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F47" s="40" t="s">
         <v>16</v>
       </c>
       <c r="G47" s="40" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H47" s="48">
         <v>21</v>
@@ -5808,244 +4904,244 @@
     </row>
     <row r="48" spans="1:9" s="57" customFormat="1">
       <c r="A48" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H48" s="56" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="I48" s="50"/>
     </row>
     <row r="49" spans="1:9" s="57" customFormat="1">
       <c r="A49" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H49" s="56" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="I49" s="50"/>
     </row>
     <row r="50" spans="1:9" ht="14">
       <c r="A50" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C50" s="7"/>
       <c r="D50" s="16"/>
       <c r="E50" s="16" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H50" s="56"/>
       <c r="I50" s="50"/>
     </row>
     <row r="51" spans="1:9" ht="14">
       <c r="A51" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H51" s="56" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I51" s="50"/>
     </row>
     <row r="52" spans="1:9" s="30" customFormat="1">
       <c r="A52" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C52" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F52" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G52" s="16" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H52" s="51" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I52" s="26"/>
     </row>
     <row r="53" spans="1:9" ht="14">
       <c r="A53" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C53" s="7"/>
       <c r="D53" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F53" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H53" s="56" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I53" s="50"/>
     </row>
     <row r="54" spans="1:9" ht="14">
       <c r="A54" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C54" s="7"/>
       <c r="D54" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H54" s="56" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="I54" s="50"/>
     </row>
     <row r="55" spans="1:9" ht="14">
       <c r="A55" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C55" s="7"/>
       <c r="D55" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F55" s="14" t="s">
         <v>16</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H55" s="56" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I55" s="50"/>
     </row>
     <row r="56" spans="1:9" ht="14">
       <c r="A56" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="7" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H56" s="56"/>
       <c r="I56" s="50"/>
     </row>
     <row r="57" spans="1:9" ht="14">
       <c r="A57" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="7" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H57" s="56">
         <v>207610</v>
@@ -6054,90 +5150,90 @@
     </row>
     <row r="58" spans="1:9" ht="14">
       <c r="A58" s="58" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B58" s="58" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C58" s="58"/>
       <c r="D58" s="58"/>
       <c r="E58" s="58" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F58" s="58" t="s">
         <v>16</v>
       </c>
       <c r="G58" s="58" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="I58" s="11"/>
     </row>
     <row r="59" spans="1:9" ht="14">
       <c r="A59" s="58" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B59" s="58" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C59" s="58"/>
       <c r="D59" s="58"/>
       <c r="E59" s="58" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F59" s="58" t="s">
         <v>16</v>
       </c>
       <c r="G59" s="58" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="I59" s="11"/>
     </row>
     <row r="60" spans="1:9" ht="14">
       <c r="A60" s="58" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B60" s="58" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C60" s="58"/>
       <c r="D60" s="58"/>
       <c r="E60" s="58" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F60" s="58" t="s">
         <v>16</v>
       </c>
       <c r="G60" s="58" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="I60" s="11"/>
     </row>
     <row r="61" spans="1:9" ht="14">
       <c r="A61" s="58" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B61" s="58" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C61" s="58"/>
       <c r="D61" s="58"/>
       <c r="E61" s="58" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F61" s="58" t="s">
         <v>16</v>
       </c>
       <c r="G61" s="58" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="H61" s="4" t="s">
         <v>18</v>
@@ -6146,45 +5242,45 @@
     </row>
     <row r="62" spans="1:9" ht="14">
       <c r="A62" s="58" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B62" s="58" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C62" s="58"/>
       <c r="D62" s="58"/>
       <c r="E62" s="58" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="F62" s="58" t="s">
         <v>16</v>
       </c>
       <c r="G62" s="58" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H62" s="4"/>
       <c r="I62" s="11"/>
     </row>
     <row r="63" spans="1:9" ht="14">
       <c r="A63" s="9" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C63" s="9"/>
       <c r="D63" s="9"/>
       <c r="E63" s="9" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F63" s="9" t="s">
         <v>16</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H63" s="38" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="I63" s="19"/>
     </row>
@@ -6201,10 +5297,10 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="49" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B65" s="20" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C65" s="24"/>
       <c r="D65" s="24"/>
@@ -6216,97 +5312,97 @@
     </row>
     <row r="66" spans="1:9" ht="14">
       <c r="A66" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
       <c r="E66" s="6" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H66" s="45" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="I66" s="15"/>
     </row>
     <row r="67" spans="1:9" ht="14">
       <c r="A67" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
       <c r="E67" s="6" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F67" s="6"/>
       <c r="G67" s="6" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="H67" s="45" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="I67" s="15"/>
     </row>
     <row r="68" spans="1:9" ht="14">
       <c r="A68" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
       <c r="E68" s="6" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="H68" s="45" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="I68" s="15"/>
     </row>
     <row r="69" spans="1:9" ht="14">
       <c r="A69" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C69" s="6"/>
       <c r="D69" s="6" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F69" s="6"/>
       <c r="G69" s="6" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H69" s="45" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="I69" s="15"/>
     </row>
     <row r="70" spans="1:9" ht="14">
       <c r="A70" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>12</v>
@@ -6318,17 +5414,17 @@
       </c>
       <c r="F70" s="6"/>
       <c r="G70" s="6" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="H70" s="45"/>
       <c r="I70" s="15"/>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B71" s="21" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C71" s="6"/>
       <c r="D71" s="21"/>
@@ -6337,17 +5433,17 @@
       </c>
       <c r="F71" s="21"/>
       <c r="G71" s="6" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H71" s="45"/>
       <c r="I71" s="15"/>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B72" s="21" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>82</v>
@@ -6358,19 +5454,19 @@
       </c>
       <c r="F72" s="21"/>
       <c r="G72" s="6" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="H72" s="45" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I72" s="15"/>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B73" s="21" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C73" s="6"/>
       <c r="D73" s="21"/>
@@ -6379,17 +5475,17 @@
       </c>
       <c r="F73" s="21"/>
       <c r="G73" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H73" s="45"/>
       <c r="I73" s="15"/>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B74" s="21" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C74" s="6"/>
       <c r="D74" s="21"/>
@@ -6398,10 +5494,10 @@
       </c>
       <c r="F74" s="21"/>
       <c r="G74" s="21" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="H74" s="45" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="I74" s="15"/>
     </row>
@@ -6415,7 +5511,7 @@
     </row>
     <row r="76" spans="1:9" ht="14">
       <c r="A76" s="42" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B76" s="62"/>
       <c r="D76" s="62"/>
@@ -6425,48 +5521,48 @@
     </row>
     <row r="77" spans="1:9" ht="14">
       <c r="A77" s="27" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B77" s="27" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C77" s="22"/>
       <c r="D77" s="27" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E77" s="22" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F77" s="27" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G77" s="27" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H77" s="52" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I77" s="11"/>
     </row>
     <row r="78" spans="1:9" ht="14">
       <c r="A78" s="27" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B78" s="27" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C78" s="22"/>
       <c r="D78" s="27" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E78" s="22" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F78" s="27" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="G78" s="27" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="H78" s="52">
         <v>2013</v>
@@ -6475,23 +5571,23 @@
     </row>
     <row r="79" spans="1:9" ht="14">
       <c r="A79" s="27" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B79" s="27" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C79" s="22"/>
       <c r="D79" s="27" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E79" s="22" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F79" s="43" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G79" s="43" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H79" s="52">
         <v>11</v>
@@ -6500,23 +5596,23 @@
     </row>
     <row r="80" spans="1:9" ht="14">
       <c r="A80" s="27" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B80" s="27" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C80" s="22"/>
       <c r="D80" s="27" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E80" s="22" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F80" s="27" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G80" s="27" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="H80" s="52">
         <v>14</v>
@@ -6528,27 +5624,26 @@
         <v>80</v>
       </c>
       <c r="B81" s="61" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C81" s="22"/>
       <c r="D81" s="61" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E81" s="22" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F81" s="61" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="G81" s="61" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="H81" s="46"/>
       <c r="I81" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6559,7 +5654,6 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6576,13 +5670,13 @@
   <sheetData>
     <row r="1" spans="1:8" s="30" customFormat="1" ht="25">
       <c r="A1" s="54" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B1" s="54" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C1" s="54" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D1" s="44" t="s">
         <v>68</v>
@@ -6591,228 +5685,228 @@
         <v>52</v>
       </c>
       <c r="F1" s="44" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G1" s="44" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H1" s="44" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
       <c r="A2" s="11" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>99</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="F2" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="G2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="H2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="11" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F3" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="G3" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="H3" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="11" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D4" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E4" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F4" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G4" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="H4" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D5" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="F5" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="G5" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="H5" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D6" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F6" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="H6" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F7" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="G7" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="F8" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="G8" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C9" s="11"/>
       <c r="F9" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="G9" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C10" s="11"/>
       <c r="F10" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="G10" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1">
       <c r="A11" s="11"/>
       <c r="B11" s="11" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C11" s="11"/>
       <c r="F11" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="G11" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="11"/>
       <c r="B12" s="11" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C12" s="11"/>
       <c r="F12" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="G12" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1">
       <c r="A13" s="11"/>
       <c r="B13" s="11" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C13" s="11"/>
       <c r="F13" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="G13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1">
@@ -6820,10 +5914,10 @@
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
       <c r="F14" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="G14" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1">
@@ -6831,10 +5925,10 @@
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
       <c r="F15" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="G15" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1">
@@ -6842,10 +5936,10 @@
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="F16" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="G16" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1">
@@ -6853,10 +5947,10 @@
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
       <c r="F17" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="G17" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1">
@@ -6864,10 +5958,10 @@
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="F18" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="G18" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1">
@@ -6875,10 +5969,10 @@
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
       <c r="F19" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="G19" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1">
@@ -6886,10 +5980,10 @@
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
       <c r="F20" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G20" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1">
@@ -6897,10 +5991,10 @@
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
       <c r="F21" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="G21" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" customHeight="1">
@@ -6908,10 +6002,10 @@
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
       <c r="F22" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="G22" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1">
@@ -6919,10 +6013,10 @@
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
       <c r="F23" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="G23" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15" customHeight="1">
@@ -6930,10 +6024,10 @@
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
       <c r="F24" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="G24" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15" customHeight="1">
@@ -6941,10 +6035,10 @@
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="F25" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G25" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1">
@@ -6952,10 +6046,10 @@
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
       <c r="F26" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="G26" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15" customHeight="1">
@@ -6963,10 +6057,10 @@
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
       <c r="F27" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="G27" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" customHeight="1">
@@ -6974,10 +6068,10 @@
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
       <c r="F28" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G28" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15" customHeight="1">
@@ -6985,10 +6079,10 @@
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
       <c r="F29" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="G29" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15" customHeight="1">
@@ -6996,10 +6090,10 @@
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
       <c r="F30" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="G30" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15" customHeight="1">
@@ -7007,10 +6101,10 @@
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
       <c r="F31" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="G31" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15" customHeight="1">
@@ -7018,10 +6112,10 @@
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
       <c r="F32" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="G32" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15" customHeight="1">
@@ -7029,10 +6123,10 @@
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
       <c r="F33" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="G33" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" customHeight="1">
@@ -7040,10 +6134,10 @@
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
       <c r="F34" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="G34" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15" customHeight="1">
@@ -7051,10 +6145,10 @@
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
       <c r="F35" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="G35" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15" customHeight="1">
@@ -7062,10 +6156,10 @@
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
       <c r="F36" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="G36" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15" customHeight="1">
@@ -7073,7 +6167,7 @@
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
       <c r="F37" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15" customHeight="1">
@@ -7081,7 +6175,7 @@
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
       <c r="F38" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15" customHeight="1">
@@ -7089,7 +6183,7 @@
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
       <c r="F39" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" customHeight="1">
@@ -7097,7 +6191,7 @@
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
       <c r="F40" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15" customHeight="1">
@@ -7105,7 +6199,7 @@
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
       <c r="F41" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15" customHeight="1">
@@ -7113,7 +6207,7 @@
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
       <c r="F42" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15" customHeight="1">
@@ -7121,7 +6215,7 @@
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
       <c r="F43" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15" customHeight="1">
@@ -7129,7 +6223,7 @@
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
       <c r="F44" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15" customHeight="1">
@@ -7137,7 +6231,7 @@
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
       <c r="F45" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15" customHeight="1">
@@ -7145,7 +6239,7 @@
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
       <c r="F46" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15" customHeight="1">
@@ -7153,7 +6247,7 @@
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
       <c r="F47" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15" customHeight="1">
@@ -7161,7 +6255,7 @@
       <c r="B48" s="11"/>
       <c r="C48" s="11"/>
       <c r="F48" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1">
@@ -7169,7 +6263,7 @@
       <c r="B49" s="11"/>
       <c r="C49" s="11"/>
       <c r="F49" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1">
@@ -7177,7 +6271,7 @@
       <c r="B50" s="11"/>
       <c r="C50" s="11"/>
       <c r="F50" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1">
@@ -7185,7 +6279,7 @@
       <c r="B51" s="11"/>
       <c r="C51" s="11"/>
       <c r="F51" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1">
@@ -7193,7 +6287,7 @@
       <c r="B52" s="11"/>
       <c r="C52" s="11"/>
       <c r="F52" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1">
@@ -7201,7 +6295,7 @@
       <c r="B53" s="11"/>
       <c r="C53" s="11"/>
       <c r="F53" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1">
@@ -7209,7 +6303,7 @@
       <c r="B54" s="11"/>
       <c r="C54" s="11"/>
       <c r="F54" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1">
@@ -7217,7 +6311,7 @@
       <c r="B55" s="11"/>
       <c r="C55" s="11"/>
       <c r="F55" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1">
@@ -7225,7 +6319,7 @@
       <c r="B56" s="11"/>
       <c r="C56" s="11"/>
       <c r="F56" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1">
@@ -7233,7 +6327,7 @@
       <c r="B57" s="11"/>
       <c r="C57" s="11"/>
       <c r="F57" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="15" customHeight="1">
@@ -7241,7 +6335,7 @@
       <c r="B58" s="11"/>
       <c r="C58" s="11"/>
       <c r="F58" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="15" customHeight="1">
@@ -7249,7 +6343,7 @@
       <c r="B59" s="11"/>
       <c r="C59" s="11"/>
       <c r="F59" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="15" customHeight="1">
@@ -7257,7 +6351,7 @@
       <c r="B60" s="11"/>
       <c r="C60" s="11"/>
       <c r="F60" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="15" customHeight="1">
@@ -7265,7 +6359,7 @@
       <c r="B61" s="11"/>
       <c r="C61" s="11"/>
       <c r="F61" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="15" customHeight="1">
@@ -7273,7 +6367,7 @@
       <c r="B62" s="11"/>
       <c r="C62" s="11"/>
       <c r="F62" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="15" customHeight="1">
@@ -7281,7 +6375,7 @@
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>
       <c r="F63" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1">
@@ -7289,7 +6383,7 @@
       <c r="B64" s="11"/>
       <c r="C64" s="11"/>
       <c r="F64" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="15" customHeight="1">
@@ -7297,7 +6391,7 @@
       <c r="B65" s="11"/>
       <c r="C65" s="11"/>
       <c r="F65" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="15" customHeight="1">
@@ -7305,7 +6399,7 @@
       <c r="B66" s="11"/>
       <c r="C66" s="11"/>
       <c r="F66" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="15" customHeight="1">
@@ -7313,7 +6407,7 @@
       <c r="B67" s="11"/>
       <c r="C67" s="11"/>
       <c r="F67" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="15" customHeight="1">
@@ -7321,7 +6415,7 @@
       <c r="B68" s="11"/>
       <c r="C68" s="11"/>
       <c r="F68" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15" customHeight="1">
@@ -7329,7 +6423,7 @@
       <c r="B69" s="11"/>
       <c r="C69" s="11"/>
       <c r="F69" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="15" customHeight="1">
@@ -7337,7 +6431,7 @@
       <c r="B70" s="11"/>
       <c r="C70" s="11"/>
       <c r="F70" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="15" customHeight="1">
@@ -7345,7 +6439,7 @@
       <c r="B71" s="11"/>
       <c r="C71" s="11"/>
       <c r="F71" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="15" customHeight="1">
@@ -7353,7 +6447,7 @@
       <c r="B72" s="11"/>
       <c r="C72" s="11"/>
       <c r="F72" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="15" customHeight="1">
@@ -7361,7 +6455,7 @@
       <c r="B73" s="11"/>
       <c r="C73" s="11"/>
       <c r="F73" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="15" customHeight="1">
@@ -7369,7 +6463,7 @@
       <c r="B74" s="11"/>
       <c r="C74" s="11"/>
       <c r="F74" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="15" customHeight="1">
@@ -7377,7 +6471,7 @@
       <c r="B75" s="11"/>
       <c r="C75" s="11"/>
       <c r="F75" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="15" customHeight="1">
@@ -7385,7 +6479,7 @@
       <c r="B76" s="11"/>
       <c r="C76" s="11"/>
       <c r="F76" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="15" customHeight="1">
@@ -7393,7 +6487,7 @@
       <c r="B77" s="11"/>
       <c r="C77" s="11"/>
       <c r="F77" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="15" customHeight="1">
@@ -7401,7 +6495,7 @@
       <c r="B78" s="11"/>
       <c r="C78" s="11"/>
       <c r="F78" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="15" customHeight="1">
@@ -7409,12 +6503,12 @@
       <c r="B79" s="11"/>
       <c r="C79" s="11"/>
       <c r="F79" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="15" customHeight="1">
       <c r="F80" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>

</xml_diff>